<commit_message>
Fixed spread calculation in chartist tool.
</commit_message>
<xml_diff>
--- a/Macro_Chartist/SavedData/bitcoin.xlsx
+++ b/Macro_Chartist/SavedData/bitcoin.xlsx
@@ -9,7 +9,6 @@
   <sheets>
     <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Closing_Price" sheetId="1" state="visible" r:id="rId1"/>
     <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="SeriesInfo" sheetId="2" state="visible" r:id="rId2"/>
-    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="OtherInfo" sheetId="3" state="visible" r:id="rId3"/>
   </sheets>
   <definedNames/>
   <calcPr calcId="124519" fullCalcOnLoad="1"/>
@@ -435,7 +434,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:B3635"/>
+  <dimension ref="A1:B3869"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -451,7 +450,7 @@
       </c>
       <c r="B1" s="1" t="inlineStr">
         <is>
-          <t>bitcoin</t>
+          <t>Trace_2</t>
         </is>
       </c>
     </row>
@@ -29519,6 +29518,1878 @@
       </c>
       <c r="B3635" t="n">
         <v>27968.12804705512</v>
+      </c>
+    </row>
+    <row r="3636">
+      <c r="A3636" s="3" t="n">
+        <v>45025</v>
+      </c>
+      <c r="B3636" t="n">
+        <v>28351.23699385011</v>
+      </c>
+    </row>
+    <row r="3637">
+      <c r="A3637" s="3" t="n">
+        <v>45026</v>
+      </c>
+      <c r="B3637" t="n">
+        <v>29657.97413687356</v>
+      </c>
+    </row>
+    <row r="3638">
+      <c r="A3638" s="3" t="n">
+        <v>45027</v>
+      </c>
+      <c r="B3638" t="n">
+        <v>30260.93610940865</v>
+      </c>
+    </row>
+    <row r="3639">
+      <c r="A3639" s="3" t="n">
+        <v>45028</v>
+      </c>
+      <c r="B3639" t="n">
+        <v>29904.13869471891</v>
+      </c>
+    </row>
+    <row r="3640">
+      <c r="A3640" s="3" t="n">
+        <v>45029</v>
+      </c>
+      <c r="B3640" t="n">
+        <v>30405.02731278115</v>
+      </c>
+    </row>
+    <row r="3641">
+      <c r="A3641" s="3" t="n">
+        <v>45030</v>
+      </c>
+      <c r="B3641" t="n">
+        <v>30468.40870059078</v>
+      </c>
+    </row>
+    <row r="3642">
+      <c r="A3642" s="3" t="n">
+        <v>45031</v>
+      </c>
+      <c r="B3642" t="n">
+        <v>30312.16187965924</v>
+      </c>
+    </row>
+    <row r="3643">
+      <c r="A3643" s="3" t="n">
+        <v>45032</v>
+      </c>
+      <c r="B3643" t="n">
+        <v>30304.80751478584</v>
+      </c>
+    </row>
+    <row r="3644">
+      <c r="A3644" s="3" t="n">
+        <v>45033</v>
+      </c>
+      <c r="B3644" t="n">
+        <v>29467.45982926034</v>
+      </c>
+    </row>
+    <row r="3645">
+      <c r="A3645" s="3" t="n">
+        <v>45034</v>
+      </c>
+      <c r="B3645" t="n">
+        <v>30365.90416754141</v>
+      </c>
+    </row>
+    <row r="3646">
+      <c r="A3646" s="3" t="n">
+        <v>45035</v>
+      </c>
+      <c r="B3646" t="n">
+        <v>28833.2175012211</v>
+      </c>
+    </row>
+    <row r="3647">
+      <c r="A3647" s="3" t="n">
+        <v>45036</v>
+      </c>
+      <c r="B3647" t="n">
+        <v>28255.57824866478</v>
+      </c>
+    </row>
+    <row r="3648">
+      <c r="A3648" s="3" t="n">
+        <v>45037</v>
+      </c>
+      <c r="B3648" t="n">
+        <v>27300.15712851557</v>
+      </c>
+    </row>
+    <row r="3649">
+      <c r="A3649" s="3" t="n">
+        <v>45038</v>
+      </c>
+      <c r="B3649" t="n">
+        <v>27861.64066347655</v>
+      </c>
+    </row>
+    <row r="3650">
+      <c r="A3650" s="3" t="n">
+        <v>45039</v>
+      </c>
+      <c r="B3650" t="n">
+        <v>27606.57834765314</v>
+      </c>
+    </row>
+    <row r="3651">
+      <c r="A3651" s="3" t="n">
+        <v>45040</v>
+      </c>
+      <c r="B3651" t="n">
+        <v>27511.63568216131</v>
+      </c>
+    </row>
+    <row r="3652">
+      <c r="A3652" s="3" t="n">
+        <v>45041</v>
+      </c>
+      <c r="B3652" t="n">
+        <v>28351.21824837301</v>
+      </c>
+    </row>
+    <row r="3653">
+      <c r="A3653" s="3" t="n">
+        <v>45042</v>
+      </c>
+      <c r="B3653" t="n">
+        <v>28352.19132059668</v>
+      </c>
+    </row>
+    <row r="3654">
+      <c r="A3654" s="3" t="n">
+        <v>45043</v>
+      </c>
+      <c r="B3654" t="n">
+        <v>29483.52170499186</v>
+      </c>
+    </row>
+    <row r="3655">
+      <c r="A3655" s="3" t="n">
+        <v>45044</v>
+      </c>
+      <c r="B3655" t="n">
+        <v>29339.99499754935</v>
+      </c>
+    </row>
+    <row r="3656">
+      <c r="A3656" s="3" t="n">
+        <v>45045</v>
+      </c>
+      <c r="B3656" t="n">
+        <v>29217.94404680991</v>
+      </c>
+    </row>
+    <row r="3657">
+      <c r="A3657" s="3" t="n">
+        <v>45046</v>
+      </c>
+      <c r="B3657" t="n">
+        <v>29362.05621362539</v>
+      </c>
+    </row>
+    <row r="3658">
+      <c r="A3658" s="3" t="n">
+        <v>45047</v>
+      </c>
+      <c r="B3658" t="n">
+        <v>28125.50115563682</v>
+      </c>
+    </row>
+    <row r="3659">
+      <c r="A3659" s="3" t="n">
+        <v>45048</v>
+      </c>
+      <c r="B3659" t="n">
+        <v>28654.39013332672</v>
+      </c>
+    </row>
+    <row r="3660">
+      <c r="A3660" s="3" t="n">
+        <v>45049</v>
+      </c>
+      <c r="B3660" t="n">
+        <v>28988.32099624927</v>
+      </c>
+    </row>
+    <row r="3661">
+      <c r="A3661" s="3" t="n">
+        <v>45050</v>
+      </c>
+      <c r="B3661" t="n">
+        <v>28846.46145860806</v>
+      </c>
+    </row>
+    <row r="3662">
+      <c r="A3662" s="3" t="n">
+        <v>45051</v>
+      </c>
+      <c r="B3662" t="n">
+        <v>29520.3222689705</v>
+      </c>
+    </row>
+    <row r="3663">
+      <c r="A3663" s="3" t="n">
+        <v>45052</v>
+      </c>
+      <c r="B3663" t="n">
+        <v>28887.74104552337</v>
+      </c>
+    </row>
+    <row r="3664">
+      <c r="A3664" s="3" t="n">
+        <v>45053</v>
+      </c>
+      <c r="B3664" t="n">
+        <v>28611.43919761457</v>
+      </c>
+    </row>
+    <row r="3665">
+      <c r="A3665" s="3" t="n">
+        <v>45054</v>
+      </c>
+      <c r="B3665" t="n">
+        <v>27696.76078562556</v>
+      </c>
+    </row>
+    <row r="3666">
+      <c r="A3666" s="3" t="n">
+        <v>45055</v>
+      </c>
+      <c r="B3666" t="n">
+        <v>27607.39168091902</v>
+      </c>
+    </row>
+    <row r="3667">
+      <c r="A3667" s="3" t="n">
+        <v>45056</v>
+      </c>
+      <c r="B3667" t="n">
+        <v>27639.73356593586</v>
+      </c>
+    </row>
+    <row r="3668">
+      <c r="A3668" s="3" t="n">
+        <v>45057</v>
+      </c>
+      <c r="B3668" t="n">
+        <v>27024.76572929978</v>
+      </c>
+    </row>
+    <row r="3669">
+      <c r="A3669" s="3" t="n">
+        <v>45058</v>
+      </c>
+      <c r="B3669" t="n">
+        <v>26787.69039591833</v>
+      </c>
+    </row>
+    <row r="3670">
+      <c r="A3670" s="3" t="n">
+        <v>45059</v>
+      </c>
+      <c r="B3670" t="n">
+        <v>26798.1262714747</v>
+      </c>
+    </row>
+    <row r="3671">
+      <c r="A3671" s="3" t="n">
+        <v>45060</v>
+      </c>
+      <c r="B3671" t="n">
+        <v>26911.80527321389</v>
+      </c>
+    </row>
+    <row r="3672">
+      <c r="A3672" s="3" t="n">
+        <v>45061</v>
+      </c>
+      <c r="B3672" t="n">
+        <v>27227.79342255879</v>
+      </c>
+    </row>
+    <row r="3673">
+      <c r="A3673" s="3" t="n">
+        <v>45062</v>
+      </c>
+      <c r="B3673" t="n">
+        <v>27022.71317392115</v>
+      </c>
+    </row>
+    <row r="3674">
+      <c r="A3674" s="3" t="n">
+        <v>45063</v>
+      </c>
+      <c r="B3674" t="n">
+        <v>27389.9715114422</v>
+      </c>
+    </row>
+    <row r="3675">
+      <c r="A3675" s="3" t="n">
+        <v>45064</v>
+      </c>
+      <c r="B3675" t="n">
+        <v>26842.95249471792</v>
+      </c>
+    </row>
+    <row r="3676">
+      <c r="A3676" s="3" t="n">
+        <v>45065</v>
+      </c>
+      <c r="B3676" t="n">
+        <v>26884.37105958995</v>
+      </c>
+    </row>
+    <row r="3677">
+      <c r="A3677" s="3" t="n">
+        <v>45066</v>
+      </c>
+      <c r="B3677" t="n">
+        <v>27093.79110149735</v>
+      </c>
+    </row>
+    <row r="3678">
+      <c r="A3678" s="3" t="n">
+        <v>45067</v>
+      </c>
+      <c r="B3678" t="n">
+        <v>26773.83024366478</v>
+      </c>
+    </row>
+    <row r="3679">
+      <c r="A3679" s="3" t="n">
+        <v>45068</v>
+      </c>
+      <c r="B3679" t="n">
+        <v>26869.68602179078</v>
+      </c>
+    </row>
+    <row r="3680">
+      <c r="A3680" s="3" t="n">
+        <v>45069</v>
+      </c>
+      <c r="B3680" t="n">
+        <v>27222.93774660385</v>
+      </c>
+    </row>
+    <row r="3681">
+      <c r="A3681" s="3" t="n">
+        <v>45070</v>
+      </c>
+      <c r="B3681" t="n">
+        <v>26338.94894699869</v>
+      </c>
+    </row>
+    <row r="3682">
+      <c r="A3682" s="3" t="n">
+        <v>45071</v>
+      </c>
+      <c r="B3682" t="n">
+        <v>26475.60790253427</v>
+      </c>
+    </row>
+    <row r="3683">
+      <c r="A3683" s="3" t="n">
+        <v>45072</v>
+      </c>
+      <c r="B3683" t="n">
+        <v>26717.98755357178</v>
+      </c>
+    </row>
+    <row r="3684">
+      <c r="A3684" s="3" t="n">
+        <v>45073</v>
+      </c>
+      <c r="B3684" t="n">
+        <v>26848.23993959246</v>
+      </c>
+    </row>
+    <row r="3685">
+      <c r="A3685" s="3" t="n">
+        <v>45074</v>
+      </c>
+      <c r="B3685" t="n">
+        <v>28110.31346760928</v>
+      </c>
+    </row>
+    <row r="3686">
+      <c r="A3686" s="3" t="n">
+        <v>45075</v>
+      </c>
+      <c r="B3686" t="n">
+        <v>27759.74666392068</v>
+      </c>
+    </row>
+    <row r="3687">
+      <c r="A3687" s="3" t="n">
+        <v>45076</v>
+      </c>
+      <c r="B3687" t="n">
+        <v>27713.90854752951</v>
+      </c>
+    </row>
+    <row r="3688">
+      <c r="A3688" s="3" t="n">
+        <v>45077</v>
+      </c>
+      <c r="B3688" t="n">
+        <v>27245.47446517972</v>
+      </c>
+    </row>
+    <row r="3689">
+      <c r="A3689" s="3" t="n">
+        <v>45078</v>
+      </c>
+      <c r="B3689" t="n">
+        <v>26824.10149951678</v>
+      </c>
+    </row>
+    <row r="3690">
+      <c r="A3690" s="3" t="n">
+        <v>45079</v>
+      </c>
+      <c r="B3690" t="n">
+        <v>27247.74008145703</v>
+      </c>
+    </row>
+    <row r="3691">
+      <c r="A3691" s="3" t="n">
+        <v>45080</v>
+      </c>
+      <c r="B3691" t="n">
+        <v>27066.37132852623</v>
+      </c>
+    </row>
+    <row r="3692">
+      <c r="A3692" s="3" t="n">
+        <v>45081</v>
+      </c>
+      <c r="B3692" t="n">
+        <v>27315.44758748768</v>
+      </c>
+    </row>
+    <row r="3693">
+      <c r="A3693" s="3" t="n">
+        <v>45082</v>
+      </c>
+      <c r="B3693" t="n">
+        <v>25792.6160902334</v>
+      </c>
+    </row>
+    <row r="3694">
+      <c r="A3694" s="3" t="n">
+        <v>45083</v>
+      </c>
+      <c r="B3694" t="n">
+        <v>27216.61556469773</v>
+      </c>
+    </row>
+    <row r="3695">
+      <c r="A3695" s="3" t="n">
+        <v>45084</v>
+      </c>
+      <c r="B3695" t="n">
+        <v>26346.24454513763</v>
+      </c>
+    </row>
+    <row r="3696">
+      <c r="A3696" s="3" t="n">
+        <v>45085</v>
+      </c>
+      <c r="B3696" t="n">
+        <v>26507.90989220298</v>
+      </c>
+    </row>
+    <row r="3697">
+      <c r="A3697" s="3" t="n">
+        <v>45086</v>
+      </c>
+      <c r="B3697" t="n">
+        <v>26469.58168400703</v>
+      </c>
+    </row>
+    <row r="3698">
+      <c r="A3698" s="3" t="n">
+        <v>45087</v>
+      </c>
+      <c r="B3698" t="n">
+        <v>25858.12289218562</v>
+      </c>
+    </row>
+    <row r="3699">
+      <c r="A3699" s="3" t="n">
+        <v>45088</v>
+      </c>
+      <c r="B3699" t="n">
+        <v>25916.57989637981</v>
+      </c>
+    </row>
+    <row r="3700">
+      <c r="A3700" s="3" t="n">
+        <v>45089</v>
+      </c>
+      <c r="B3700" t="n">
+        <v>25910.36274291946</v>
+      </c>
+    </row>
+    <row r="3701">
+      <c r="A3701" s="3" t="n">
+        <v>45090</v>
+      </c>
+      <c r="B3701" t="n">
+        <v>25872.20645879509</v>
+      </c>
+    </row>
+    <row r="3702">
+      <c r="A3702" s="3" t="n">
+        <v>45091</v>
+      </c>
+      <c r="B3702" t="n">
+        <v>25107.75469588059</v>
+      </c>
+    </row>
+    <row r="3703">
+      <c r="A3703" s="3" t="n">
+        <v>45092</v>
+      </c>
+      <c r="B3703" t="n">
+        <v>25564.59963288714</v>
+      </c>
+    </row>
+    <row r="3704">
+      <c r="A3704" s="3" t="n">
+        <v>45093</v>
+      </c>
+      <c r="B3704" t="n">
+        <v>26327.3256694539</v>
+      </c>
+    </row>
+    <row r="3705">
+      <c r="A3705" s="3" t="n">
+        <v>45094</v>
+      </c>
+      <c r="B3705" t="n">
+        <v>26501.04444223367</v>
+      </c>
+    </row>
+    <row r="3706">
+      <c r="A3706" s="3" t="n">
+        <v>45095</v>
+      </c>
+      <c r="B3706" t="n">
+        <v>26333.09252966437</v>
+      </c>
+    </row>
+    <row r="3707">
+      <c r="A3707" s="3" t="n">
+        <v>45096</v>
+      </c>
+      <c r="B3707" t="n">
+        <v>26779.38746152284</v>
+      </c>
+    </row>
+    <row r="3708">
+      <c r="A3708" s="3" t="n">
+        <v>45097</v>
+      </c>
+      <c r="B3708" t="n">
+        <v>28330.89141980751</v>
+      </c>
+    </row>
+    <row r="3709">
+      <c r="A3709" s="3" t="n">
+        <v>45098</v>
+      </c>
+      <c r="B3709" t="n">
+        <v>30101.76481948869</v>
+      </c>
+    </row>
+    <row r="3710">
+      <c r="A3710" s="3" t="n">
+        <v>45099</v>
+      </c>
+      <c r="B3710" t="n">
+        <v>29935.63210674956</v>
+      </c>
+    </row>
+    <row r="3711">
+      <c r="A3711" s="3" t="n">
+        <v>45100</v>
+      </c>
+      <c r="B3711" t="n">
+        <v>30629.24435333575</v>
+      </c>
+    </row>
+    <row r="3712">
+      <c r="A3712" s="3" t="n">
+        <v>45101</v>
+      </c>
+      <c r="B3712" t="n">
+        <v>30537.81666463479</v>
+      </c>
+    </row>
+    <row r="3713">
+      <c r="A3713" s="3" t="n">
+        <v>45102</v>
+      </c>
+      <c r="B3713" t="n">
+        <v>30454.75697441562</v>
+      </c>
+    </row>
+    <row r="3714">
+      <c r="A3714" s="3" t="n">
+        <v>45103</v>
+      </c>
+      <c r="B3714" t="n">
+        <v>30285.50506407074</v>
+      </c>
+    </row>
+    <row r="3715">
+      <c r="A3715" s="3" t="n">
+        <v>45104</v>
+      </c>
+      <c r="B3715" t="n">
+        <v>30693.54635606798</v>
+      </c>
+    </row>
+    <row r="3716">
+      <c r="A3716" s="3" t="n">
+        <v>45105</v>
+      </c>
+      <c r="B3716" t="n">
+        <v>30083.47724526382</v>
+      </c>
+    </row>
+    <row r="3717">
+      <c r="A3717" s="3" t="n">
+        <v>45106</v>
+      </c>
+      <c r="B3717" t="n">
+        <v>30466.61045689353</v>
+      </c>
+    </row>
+    <row r="3718">
+      <c r="A3718" s="3" t="n">
+        <v>45107</v>
+      </c>
+      <c r="B3718" t="n">
+        <v>30480.78148194446</v>
+      </c>
+    </row>
+    <row r="3719">
+      <c r="A3719" s="3" t="n">
+        <v>45108</v>
+      </c>
+      <c r="B3719" t="n">
+        <v>30583.61959969754</v>
+      </c>
+    </row>
+    <row r="3720">
+      <c r="A3720" s="3" t="n">
+        <v>45109</v>
+      </c>
+      <c r="B3720" t="n">
+        <v>30571.88707287145</v>
+      </c>
+    </row>
+    <row r="3721">
+      <c r="A3721" s="3" t="n">
+        <v>45110</v>
+      </c>
+      <c r="B3721" t="n">
+        <v>31134.71313350841</v>
+      </c>
+    </row>
+    <row r="3722">
+      <c r="A3722" s="3" t="n">
+        <v>45111</v>
+      </c>
+      <c r="B3722" t="n">
+        <v>30775.6240223753</v>
+      </c>
+    </row>
+    <row r="3723">
+      <c r="A3723" s="3" t="n">
+        <v>45112</v>
+      </c>
+      <c r="B3723" t="n">
+        <v>30484.79377442352</v>
+      </c>
+    </row>
+    <row r="3724">
+      <c r="A3724" s="3" t="n">
+        <v>45113</v>
+      </c>
+      <c r="B3724" t="n">
+        <v>29990.05515122025</v>
+      </c>
+    </row>
+    <row r="3725">
+      <c r="A3725" s="3" t="n">
+        <v>45114</v>
+      </c>
+      <c r="B3725" t="n">
+        <v>30315.26540235163</v>
+      </c>
+    </row>
+    <row r="3726">
+      <c r="A3726" s="3" t="n">
+        <v>45115</v>
+      </c>
+      <c r="B3726" t="n">
+        <v>30264.19734525722</v>
+      </c>
+    </row>
+    <row r="3727">
+      <c r="A3727" s="3" t="n">
+        <v>45116</v>
+      </c>
+      <c r="B3727" t="n">
+        <v>30169.87065747925</v>
+      </c>
+    </row>
+    <row r="3728">
+      <c r="A3728" s="3" t="n">
+        <v>45117</v>
+      </c>
+      <c r="B3728" t="n">
+        <v>30394.28114637557</v>
+      </c>
+    </row>
+    <row r="3729">
+      <c r="A3729" s="3" t="n">
+        <v>45118</v>
+      </c>
+      <c r="B3729" t="n">
+        <v>30620.81424697801</v>
+      </c>
+    </row>
+    <row r="3730">
+      <c r="A3730" s="3" t="n">
+        <v>45119</v>
+      </c>
+      <c r="B3730" t="n">
+        <v>30407.41631435991</v>
+      </c>
+    </row>
+    <row r="3731">
+      <c r="A3731" s="3" t="n">
+        <v>45120</v>
+      </c>
+      <c r="B3731" t="n">
+        <v>31446.0149710716</v>
+      </c>
+    </row>
+    <row r="3732">
+      <c r="A3732" s="3" t="n">
+        <v>45121</v>
+      </c>
+      <c r="B3732" t="n">
+        <v>30311.82780813052</v>
+      </c>
+    </row>
+    <row r="3733">
+      <c r="A3733" s="3" t="n">
+        <v>45122</v>
+      </c>
+      <c r="B3733" t="n">
+        <v>30297.97140012553</v>
+      </c>
+    </row>
+    <row r="3734">
+      <c r="A3734" s="3" t="n">
+        <v>45123</v>
+      </c>
+      <c r="B3734" t="n">
+        <v>30237.3347851461</v>
+      </c>
+    </row>
+    <row r="3735">
+      <c r="A3735" s="3" t="n">
+        <v>45124</v>
+      </c>
+      <c r="B3735" t="n">
+        <v>30147.86007921152</v>
+      </c>
+    </row>
+    <row r="3736">
+      <c r="A3736" s="3" t="n">
+        <v>45125</v>
+      </c>
+      <c r="B3736" t="n">
+        <v>29848.03227250528</v>
+      </c>
+    </row>
+    <row r="3737">
+      <c r="A3737" s="3" t="n">
+        <v>45126</v>
+      </c>
+      <c r="B3737" t="n">
+        <v>29919.87483825516</v>
+      </c>
+    </row>
+    <row r="3738">
+      <c r="A3738" s="3" t="n">
+        <v>45127</v>
+      </c>
+      <c r="B3738" t="n">
+        <v>29787.04153035569</v>
+      </c>
+    </row>
+    <row r="3739">
+      <c r="A3739" s="3" t="n">
+        <v>45128</v>
+      </c>
+      <c r="B3739" t="n">
+        <v>29914.68272835899</v>
+      </c>
+    </row>
+    <row r="3740">
+      <c r="A3740" s="3" t="n">
+        <v>45129</v>
+      </c>
+      <c r="B3740" t="n">
+        <v>29710.15593599177</v>
+      </c>
+    </row>
+    <row r="3741">
+      <c r="A3741" s="3" t="n">
+        <v>45130</v>
+      </c>
+      <c r="B3741" t="n">
+        <v>30057.95671871459</v>
+      </c>
+    </row>
+    <row r="3742">
+      <c r="A3742" s="3" t="n">
+        <v>45131</v>
+      </c>
+      <c r="B3742" t="n">
+        <v>29184.90191305769</v>
+      </c>
+    </row>
+    <row r="3743">
+      <c r="A3743" s="3" t="n">
+        <v>45132</v>
+      </c>
+      <c r="B3743" t="n">
+        <v>29222.97463038353</v>
+      </c>
+    </row>
+    <row r="3744">
+      <c r="A3744" s="3" t="n">
+        <v>45133</v>
+      </c>
+      <c r="B3744" t="n">
+        <v>29363.67290797862</v>
+      </c>
+    </row>
+    <row r="3745">
+      <c r="A3745" s="3" t="n">
+        <v>45134</v>
+      </c>
+      <c r="B3745" t="n">
+        <v>29200.24400129131</v>
+      </c>
+    </row>
+    <row r="3746">
+      <c r="A3746" s="3" t="n">
+        <v>45135</v>
+      </c>
+      <c r="B3746" t="n">
+        <v>29314.09738709836</v>
+      </c>
+    </row>
+    <row r="3747">
+      <c r="A3747" s="3" t="n">
+        <v>45136</v>
+      </c>
+      <c r="B3747" t="n">
+        <v>29356.74774591667</v>
+      </c>
+    </row>
+    <row r="3748">
+      <c r="A3748" s="3" t="n">
+        <v>45137</v>
+      </c>
+      <c r="B3748" t="n">
+        <v>29277.75581027272</v>
+      </c>
+    </row>
+    <row r="3749">
+      <c r="A3749" s="3" t="n">
+        <v>45138</v>
+      </c>
+      <c r="B3749" t="n">
+        <v>29233.13636558044</v>
+      </c>
+    </row>
+    <row r="3750">
+      <c r="A3750" s="3" t="n">
+        <v>45139</v>
+      </c>
+      <c r="B3750" t="n">
+        <v>29537.10974692743</v>
+      </c>
+    </row>
+    <row r="3751">
+      <c r="A3751" s="3" t="n">
+        <v>45140</v>
+      </c>
+      <c r="B3751" t="n">
+        <v>29146.63627084363</v>
+      </c>
+    </row>
+    <row r="3752">
+      <c r="A3752" s="3" t="n">
+        <v>45141</v>
+      </c>
+      <c r="B3752" t="n">
+        <v>29176.15059658541</v>
+      </c>
+    </row>
+    <row r="3753">
+      <c r="A3753" s="3" t="n">
+        <v>45142</v>
+      </c>
+      <c r="B3753" t="n">
+        <v>29087.93808600763</v>
+      </c>
+    </row>
+    <row r="3754">
+      <c r="A3754" s="3" t="n">
+        <v>45143</v>
+      </c>
+      <c r="B3754" t="n">
+        <v>29046.8004570232</v>
+      </c>
+    </row>
+    <row r="3755">
+      <c r="A3755" s="3" t="n">
+        <v>45144</v>
+      </c>
+      <c r="B3755" t="n">
+        <v>29044.20437557756</v>
+      </c>
+    </row>
+    <row r="3756">
+      <c r="A3756" s="3" t="n">
+        <v>45145</v>
+      </c>
+      <c r="B3756" t="n">
+        <v>29178.14775187308</v>
+      </c>
+    </row>
+    <row r="3757">
+      <c r="A3757" s="3" t="n">
+        <v>45146</v>
+      </c>
+      <c r="B3757" t="n">
+        <v>29779.56167125089</v>
+      </c>
+    </row>
+    <row r="3758">
+      <c r="A3758" s="3" t="n">
+        <v>45147</v>
+      </c>
+      <c r="B3758" t="n">
+        <v>29585.48807737921</v>
+      </c>
+    </row>
+    <row r="3759">
+      <c r="A3759" s="3" t="n">
+        <v>45148</v>
+      </c>
+      <c r="B3759" t="n">
+        <v>29423.81891597763</v>
+      </c>
+    </row>
+    <row r="3760">
+      <c r="A3760" s="3" t="n">
+        <v>45149</v>
+      </c>
+      <c r="B3760" t="n">
+        <v>29396.8479714205</v>
+      </c>
+    </row>
+    <row r="3761">
+      <c r="A3761" s="3" t="n">
+        <v>45150</v>
+      </c>
+      <c r="B3761" t="n">
+        <v>29412.1422745841</v>
+      </c>
+    </row>
+    <row r="3762">
+      <c r="A3762" s="3" t="n">
+        <v>45151</v>
+      </c>
+      <c r="B3762" t="n">
+        <v>29284.96971374381</v>
+      </c>
+    </row>
+    <row r="3763">
+      <c r="A3763" s="3" t="n">
+        <v>45152</v>
+      </c>
+      <c r="B3763" t="n">
+        <v>29400.58680419105</v>
+      </c>
+    </row>
+    <row r="3764">
+      <c r="A3764" s="3" t="n">
+        <v>45153</v>
+      </c>
+      <c r="B3764" t="n">
+        <v>29170.49039706061</v>
+      </c>
+    </row>
+    <row r="3765">
+      <c r="A3765" s="3" t="n">
+        <v>45154</v>
+      </c>
+      <c r="B3765" t="n">
+        <v>28754.19702111257</v>
+      </c>
+    </row>
+    <row r="3766">
+      <c r="A3766" s="3" t="n">
+        <v>45155</v>
+      </c>
+      <c r="B3766" t="n">
+        <v>26501.58726991974</v>
+      </c>
+    </row>
+    <row r="3767">
+      <c r="A3767" s="3" t="n">
+        <v>45156</v>
+      </c>
+      <c r="B3767" t="n">
+        <v>26042.838256849</v>
+      </c>
+    </row>
+    <row r="3768">
+      <c r="A3768" s="3" t="n">
+        <v>45157</v>
+      </c>
+      <c r="B3768" t="n">
+        <v>26104.7786307979</v>
+      </c>
+    </row>
+    <row r="3769">
+      <c r="A3769" s="3" t="n">
+        <v>45158</v>
+      </c>
+      <c r="B3769" t="n">
+        <v>26160.70041981821</v>
+      </c>
+    </row>
+    <row r="3770">
+      <c r="A3770" s="3" t="n">
+        <v>45159</v>
+      </c>
+      <c r="B3770" t="n">
+        <v>26119.00595859522</v>
+      </c>
+    </row>
+    <row r="3771">
+      <c r="A3771" s="3" t="n">
+        <v>45160</v>
+      </c>
+      <c r="B3771" t="n">
+        <v>26033.67540658584</v>
+      </c>
+    </row>
+    <row r="3772">
+      <c r="A3772" s="3" t="n">
+        <v>45161</v>
+      </c>
+      <c r="B3772" t="n">
+        <v>26450.00862461353</v>
+      </c>
+    </row>
+    <row r="3773">
+      <c r="A3773" s="3" t="n">
+        <v>45162</v>
+      </c>
+      <c r="B3773" t="n">
+        <v>26134.934254516</v>
+      </c>
+    </row>
+    <row r="3774">
+      <c r="A3774" s="3" t="n">
+        <v>45163</v>
+      </c>
+      <c r="B3774" t="n">
+        <v>26044.03620928913</v>
+      </c>
+    </row>
+    <row r="3775">
+      <c r="A3775" s="3" t="n">
+        <v>45164</v>
+      </c>
+      <c r="B3775" t="n">
+        <v>26002.01571731937</v>
+      </c>
+    </row>
+    <row r="3776">
+      <c r="A3776" s="3" t="n">
+        <v>45165</v>
+      </c>
+      <c r="B3776" t="n">
+        <v>26082.71717821853</v>
+      </c>
+    </row>
+    <row r="3777">
+      <c r="A3777" s="3" t="n">
+        <v>45166</v>
+      </c>
+      <c r="B3777" t="n">
+        <v>26109.2698239287</v>
+      </c>
+    </row>
+    <row r="3778">
+      <c r="A3778" s="3" t="n">
+        <v>45167</v>
+      </c>
+      <c r="B3778" t="n">
+        <v>27730.50373550554</v>
+      </c>
+    </row>
+    <row r="3779">
+      <c r="A3779" s="3" t="n">
+        <v>45168</v>
+      </c>
+      <c r="B3779" t="n">
+        <v>27297.2614384804</v>
+      </c>
+    </row>
+    <row r="3780">
+      <c r="A3780" s="3" t="n">
+        <v>45169</v>
+      </c>
+      <c r="B3780" t="n">
+        <v>25927.41700577929</v>
+      </c>
+    </row>
+    <row r="3781">
+      <c r="A3781" s="3" t="n">
+        <v>45170</v>
+      </c>
+      <c r="B3781" t="n">
+        <v>25812.33049442542</v>
+      </c>
+    </row>
+    <row r="3782">
+      <c r="A3782" s="3" t="n">
+        <v>45171</v>
+      </c>
+      <c r="B3782" t="n">
+        <v>25853.65684277757</v>
+      </c>
+    </row>
+    <row r="3783">
+      <c r="A3783" s="3" t="n">
+        <v>45172</v>
+      </c>
+      <c r="B3783" t="n">
+        <v>25959.59631146345</v>
+      </c>
+    </row>
+    <row r="3784">
+      <c r="A3784" s="3" t="n">
+        <v>45173</v>
+      </c>
+      <c r="B3784" t="n">
+        <v>25829.36477294132</v>
+      </c>
+    </row>
+    <row r="3785">
+      <c r="A3785" s="3" t="n">
+        <v>45174</v>
+      </c>
+      <c r="B3785" t="n">
+        <v>25784.41351983038</v>
+      </c>
+    </row>
+    <row r="3786">
+      <c r="A3786" s="3" t="n">
+        <v>45175</v>
+      </c>
+      <c r="B3786" t="n">
+        <v>25752.95841858941</v>
+      </c>
+    </row>
+    <row r="3787">
+      <c r="A3787" s="3" t="n">
+        <v>45176</v>
+      </c>
+      <c r="B3787" t="n">
+        <v>26192.33343309057</v>
+      </c>
+    </row>
+    <row r="3788">
+      <c r="A3788" s="3" t="n">
+        <v>45177</v>
+      </c>
+      <c r="B3788" t="n">
+        <v>25907.22813724973</v>
+      </c>
+    </row>
+    <row r="3789">
+      <c r="A3789" s="3" t="n">
+        <v>45178</v>
+      </c>
+      <c r="B3789" t="n">
+        <v>25889.3250094629</v>
+      </c>
+    </row>
+    <row r="3790">
+      <c r="A3790" s="3" t="n">
+        <v>45179</v>
+      </c>
+      <c r="B3790" t="n">
+        <v>25834.58009856291</v>
+      </c>
+    </row>
+    <row r="3791">
+      <c r="A3791" s="3" t="n">
+        <v>45180</v>
+      </c>
+      <c r="B3791" t="n">
+        <v>25133.30310656653</v>
+      </c>
+    </row>
+    <row r="3792">
+      <c r="A3792" s="3" t="n">
+        <v>45181</v>
+      </c>
+      <c r="B3792" t="n">
+        <v>25866.80666315808</v>
+      </c>
+    </row>
+    <row r="3793">
+      <c r="A3793" s="3" t="n">
+        <v>45182</v>
+      </c>
+      <c r="B3793" t="n">
+        <v>26223.43607566095</v>
+      </c>
+    </row>
+    <row r="3794">
+      <c r="A3794" s="3" t="n">
+        <v>45183</v>
+      </c>
+      <c r="B3794" t="n">
+        <v>26531.39556626326</v>
+      </c>
+    </row>
+    <row r="3795">
+      <c r="A3795" s="3" t="n">
+        <v>45184</v>
+      </c>
+      <c r="B3795" t="n">
+        <v>26634.63102500059</v>
+      </c>
+    </row>
+    <row r="3796">
+      <c r="A3796" s="3" t="n">
+        <v>45185</v>
+      </c>
+      <c r="B3796" t="n">
+        <v>26557.76869199465</v>
+      </c>
+    </row>
+    <row r="3797">
+      <c r="A3797" s="3" t="n">
+        <v>45186</v>
+      </c>
+      <c r="B3797" t="n">
+        <v>26520.98825478389</v>
+      </c>
+    </row>
+    <row r="3798">
+      <c r="A3798" s="3" t="n">
+        <v>45187</v>
+      </c>
+      <c r="B3798" t="n">
+        <v>26741.46111094895</v>
+      </c>
+    </row>
+    <row r="3799">
+      <c r="A3799" s="3" t="n">
+        <v>45188</v>
+      </c>
+      <c r="B3799" t="n">
+        <v>27219.29687463422</v>
+      </c>
+    </row>
+    <row r="3800">
+      <c r="A3800" s="3" t="n">
+        <v>45189</v>
+      </c>
+      <c r="B3800" t="n">
+        <v>27115.84644697082</v>
+      </c>
+    </row>
+    <row r="3801">
+      <c r="A3801" s="3" t="n">
+        <v>45190</v>
+      </c>
+      <c r="B3801" t="n">
+        <v>26561.13345419872</v>
+      </c>
+    </row>
+    <row r="3802">
+      <c r="A3802" s="3" t="n">
+        <v>45191</v>
+      </c>
+      <c r="B3802" t="n">
+        <v>26572.0381115526</v>
+      </c>
+    </row>
+    <row r="3803">
+      <c r="A3803" s="3" t="n">
+        <v>45192</v>
+      </c>
+      <c r="B3803" t="n">
+        <v>26573.9234797301</v>
+      </c>
+    </row>
+    <row r="3804">
+      <c r="A3804" s="3" t="n">
+        <v>45193</v>
+      </c>
+      <c r="B3804" t="n">
+        <v>26249.5628978452</v>
+      </c>
+    </row>
+    <row r="3805">
+      <c r="A3805" s="3" t="n">
+        <v>45194</v>
+      </c>
+      <c r="B3805" t="n">
+        <v>26298.63467828123</v>
+      </c>
+    </row>
+    <row r="3806">
+      <c r="A3806" s="3" t="n">
+        <v>45195</v>
+      </c>
+      <c r="B3806" t="n">
+        <v>26204.75759083597</v>
+      </c>
+    </row>
+    <row r="3807">
+      <c r="A3807" s="3" t="n">
+        <v>45196</v>
+      </c>
+      <c r="B3807" t="n">
+        <v>26350.14689542806</v>
+      </c>
+    </row>
+    <row r="3808">
+      <c r="A3808" s="3" t="n">
+        <v>45197</v>
+      </c>
+      <c r="B3808" t="n">
+        <v>27009.01375072488</v>
+      </c>
+    </row>
+    <row r="3809">
+      <c r="A3809" s="3" t="n">
+        <v>45198</v>
+      </c>
+      <c r="B3809" t="n">
+        <v>26917.19910163798</v>
+      </c>
+    </row>
+    <row r="3810">
+      <c r="A3810" s="3" t="n">
+        <v>45199</v>
+      </c>
+      <c r="B3810" t="n">
+        <v>26969.87614407258</v>
+      </c>
+    </row>
+    <row r="3811">
+      <c r="A3811" s="3" t="n">
+        <v>45200</v>
+      </c>
+      <c r="B3811" t="n">
+        <v>27967.51057908711</v>
+      </c>
+    </row>
+    <row r="3812">
+      <c r="A3812" s="3" t="n">
+        <v>45201</v>
+      </c>
+      <c r="B3812" t="n">
+        <v>27615.06488509527</v>
+      </c>
+    </row>
+    <row r="3813">
+      <c r="A3813" s="3" t="n">
+        <v>45202</v>
+      </c>
+      <c r="B3813" t="n">
+        <v>27439.12194670512</v>
+      </c>
+    </row>
+    <row r="3814">
+      <c r="A3814" s="3" t="n">
+        <v>45203</v>
+      </c>
+      <c r="B3814" t="n">
+        <v>27792.1112772493</v>
+      </c>
+    </row>
+    <row r="3815">
+      <c r="A3815" s="3" t="n">
+        <v>45204</v>
+      </c>
+      <c r="B3815" t="n">
+        <v>27435.8746151351</v>
+      </c>
+    </row>
+    <row r="3816">
+      <c r="A3816" s="3" t="n">
+        <v>45205</v>
+      </c>
+      <c r="B3816" t="n">
+        <v>27958.19643735049</v>
+      </c>
+    </row>
+    <row r="3817">
+      <c r="A3817" s="3" t="n">
+        <v>45206</v>
+      </c>
+      <c r="B3817" t="n">
+        <v>27977.54349070001</v>
+      </c>
+    </row>
+    <row r="3818">
+      <c r="A3818" s="3" t="n">
+        <v>45207</v>
+      </c>
+      <c r="B3818" t="n">
+        <v>27948.10365174851</v>
+      </c>
+    </row>
+    <row r="3819">
+      <c r="A3819" s="3" t="n">
+        <v>45208</v>
+      </c>
+      <c r="B3819" t="n">
+        <v>27593.78253443967</v>
+      </c>
+    </row>
+    <row r="3820">
+      <c r="A3820" s="3" t="n">
+        <v>45209</v>
+      </c>
+      <c r="B3820" t="n">
+        <v>27392.2477027325</v>
+      </c>
+    </row>
+    <row r="3821">
+      <c r="A3821" s="3" t="n">
+        <v>45210</v>
+      </c>
+      <c r="B3821" t="n">
+        <v>26842.1904390924</v>
+      </c>
+    </row>
+    <row r="3822">
+      <c r="A3822" s="3" t="n">
+        <v>45211</v>
+      </c>
+      <c r="B3822" t="n">
+        <v>26729.13720581511</v>
+      </c>
+    </row>
+    <row r="3823">
+      <c r="A3823" s="3" t="n">
+        <v>45212</v>
+      </c>
+      <c r="B3823" t="n">
+        <v>26841.13622064441</v>
+      </c>
+    </row>
+    <row r="3824">
+      <c r="A3824" s="3" t="n">
+        <v>45213</v>
+      </c>
+      <c r="B3824" t="n">
+        <v>26863.18356907992</v>
+      </c>
+    </row>
+    <row r="3825">
+      <c r="A3825" s="3" t="n">
+        <v>45214</v>
+      </c>
+      <c r="B3825" t="n">
+        <v>27150.29700140705</v>
+      </c>
+    </row>
+    <row r="3826">
+      <c r="A3826" s="3" t="n">
+        <v>45215</v>
+      </c>
+      <c r="B3826" t="n">
+        <v>28513.30993247735</v>
+      </c>
+    </row>
+    <row r="3827">
+      <c r="A3827" s="3" t="n">
+        <v>45216</v>
+      </c>
+      <c r="B3827" t="n">
+        <v>28417.72175169982</v>
+      </c>
+    </row>
+    <row r="3828">
+      <c r="A3828" s="3" t="n">
+        <v>45217</v>
+      </c>
+      <c r="B3828" t="n">
+        <v>28328.24519813482</v>
+      </c>
+    </row>
+    <row r="3829">
+      <c r="A3829" s="3" t="n">
+        <v>45218</v>
+      </c>
+      <c r="B3829" t="n">
+        <v>28715.74814240795</v>
+      </c>
+    </row>
+    <row r="3830">
+      <c r="A3830" s="3" t="n">
+        <v>45219</v>
+      </c>
+      <c r="B3830" t="n">
+        <v>29677.39288847621</v>
+      </c>
+    </row>
+    <row r="3831">
+      <c r="A3831" s="3" t="n">
+        <v>45220</v>
+      </c>
+      <c r="B3831" t="n">
+        <v>29920.07449265145</v>
+      </c>
+    </row>
+    <row r="3832">
+      <c r="A3832" s="3" t="n">
+        <v>45221</v>
+      </c>
+      <c r="B3832" t="n">
+        <v>30019.38050086351</v>
+      </c>
+    </row>
+    <row r="3833">
+      <c r="A3833" s="3" t="n">
+        <v>45222</v>
+      </c>
+      <c r="B3833" t="n">
+        <v>32953.26276083098</v>
+      </c>
+    </row>
+    <row r="3834">
+      <c r="A3834" s="3" t="n">
+        <v>45223</v>
+      </c>
+      <c r="B3834" t="n">
+        <v>33846.72425733224</v>
+      </c>
+    </row>
+    <row r="3835">
+      <c r="A3835" s="3" t="n">
+        <v>45224</v>
+      </c>
+      <c r="B3835" t="n">
+        <v>34471.98603167202</v>
+      </c>
+    </row>
+    <row r="3836">
+      <c r="A3836" s="3" t="n">
+        <v>45225</v>
+      </c>
+      <c r="B3836" t="n">
+        <v>34174.45155291259</v>
+      </c>
+    </row>
+    <row r="3837">
+      <c r="A3837" s="3" t="n">
+        <v>45226</v>
+      </c>
+      <c r="B3837" t="n">
+        <v>33899.09305644032</v>
+      </c>
+    </row>
+    <row r="3838">
+      <c r="A3838" s="3" t="n">
+        <v>45227</v>
+      </c>
+      <c r="B3838" t="n">
+        <v>34092.63093283858</v>
+      </c>
+    </row>
+    <row r="3839">
+      <c r="A3839" s="3" t="n">
+        <v>45228</v>
+      </c>
+      <c r="B3839" t="n">
+        <v>34556.24281476162</v>
+      </c>
+    </row>
+    <row r="3840">
+      <c r="A3840" s="3" t="n">
+        <v>45229</v>
+      </c>
+      <c r="B3840" t="n">
+        <v>34498.70391946407</v>
+      </c>
+    </row>
+    <row r="3841">
+      <c r="A3841" s="3" t="n">
+        <v>45230</v>
+      </c>
+      <c r="B3841" t="n">
+        <v>34672.2892841885</v>
+      </c>
+    </row>
+    <row r="3842">
+      <c r="A3842" s="3" t="n">
+        <v>45231</v>
+      </c>
+      <c r="B3842" t="n">
+        <v>35457.45491210553</v>
+      </c>
+    </row>
+    <row r="3843">
+      <c r="A3843" s="3" t="n">
+        <v>45232</v>
+      </c>
+      <c r="B3843" t="n">
+        <v>34924.05545044328</v>
+      </c>
+    </row>
+    <row r="3844">
+      <c r="A3844" s="3" t="n">
+        <v>45233</v>
+      </c>
+      <c r="B3844" t="n">
+        <v>34731.38136896784</v>
+      </c>
+    </row>
+    <row r="3845">
+      <c r="A3845" s="3" t="n">
+        <v>45234</v>
+      </c>
+      <c r="B3845" t="n">
+        <v>35048.40783490107</v>
+      </c>
+    </row>
+    <row r="3846">
+      <c r="A3846" s="3" t="n">
+        <v>45235</v>
+      </c>
+      <c r="B3846" t="n">
+        <v>35061.92874919579</v>
+      </c>
+    </row>
+    <row r="3847">
+      <c r="A3847" s="3" t="n">
+        <v>45236</v>
+      </c>
+      <c r="B3847" t="n">
+        <v>35031.26888208706</v>
+      </c>
+    </row>
+    <row r="3848">
+      <c r="A3848" s="3" t="n">
+        <v>45237</v>
+      </c>
+      <c r="B3848" t="n">
+        <v>35436.53762957962</v>
+      </c>
+    </row>
+    <row r="3849">
+      <c r="A3849" s="3" t="n">
+        <v>45238</v>
+      </c>
+      <c r="B3849" t="n">
+        <v>35795.0806307102</v>
+      </c>
+    </row>
+    <row r="3850">
+      <c r="A3850" s="3" t="n">
+        <v>45239</v>
+      </c>
+      <c r="B3850" t="n">
+        <v>36768.42081912672</v>
+      </c>
+    </row>
+    <row r="3851">
+      <c r="A3851" s="3" t="n">
+        <v>45240</v>
+      </c>
+      <c r="B3851" t="n">
+        <v>37344.24900072035</v>
+      </c>
+    </row>
+    <row r="3852">
+      <c r="A3852" s="3" t="n">
+        <v>45241</v>
+      </c>
+      <c r="B3852" t="n">
+        <v>37122.72282430655</v>
+      </c>
+    </row>
+    <row r="3853">
+      <c r="A3853" s="3" t="n">
+        <v>45242</v>
+      </c>
+      <c r="B3853" t="n">
+        <v>37067.69698212008</v>
+      </c>
+    </row>
+    <row r="3854">
+      <c r="A3854" s="3" t="n">
+        <v>45243</v>
+      </c>
+      <c r="B3854" t="n">
+        <v>36549.16204829837</v>
+      </c>
+    </row>
+    <row r="3855">
+      <c r="A3855" s="3" t="n">
+        <v>45244</v>
+      </c>
+      <c r="B3855" t="n">
+        <v>35545.20143345407</v>
+      </c>
+    </row>
+    <row r="3856">
+      <c r="A3856" s="3" t="n">
+        <v>45245</v>
+      </c>
+      <c r="B3856" t="n">
+        <v>37903.66245166294</v>
+      </c>
+    </row>
+    <row r="3857">
+      <c r="A3857" s="3" t="n">
+        <v>45246</v>
+      </c>
+      <c r="B3857" t="n">
+        <v>36201.51611146142</v>
+      </c>
+    </row>
+    <row r="3858">
+      <c r="A3858" s="3" t="n">
+        <v>45247</v>
+      </c>
+      <c r="B3858" t="n">
+        <v>36527.76022530742</v>
+      </c>
+    </row>
+    <row r="3859">
+      <c r="A3859" s="3" t="n">
+        <v>45248</v>
+      </c>
+      <c r="B3859" t="n">
+        <v>36582.36844192274</v>
+      </c>
+    </row>
+    <row r="3860">
+      <c r="A3860" s="3" t="n">
+        <v>45249</v>
+      </c>
+      <c r="B3860" t="n">
+        <v>37413.99460790531</v>
+      </c>
+    </row>
+    <row r="3861">
+      <c r="A3861" s="3" t="n">
+        <v>45250</v>
+      </c>
+      <c r="B3861" t="n">
+        <v>37489.29847080202</v>
+      </c>
+    </row>
+    <row r="3862">
+      <c r="A3862" s="3" t="n">
+        <v>45251</v>
+      </c>
+      <c r="B3862" t="n">
+        <v>35965.36036068078</v>
+      </c>
+    </row>
+    <row r="3863">
+      <c r="A3863" s="3" t="n">
+        <v>45252</v>
+      </c>
+      <c r="B3863" t="n">
+        <v>37464.83293220907</v>
+      </c>
+    </row>
+    <row r="3864">
+      <c r="A3864" s="3" t="n">
+        <v>45253</v>
+      </c>
+      <c r="B3864" t="n">
+        <v>37293.31612742673</v>
+      </c>
+    </row>
+    <row r="3865">
+      <c r="A3865" s="3" t="n">
+        <v>45254</v>
+      </c>
+      <c r="B3865" t="n">
+        <v>37738.93169747125</v>
+      </c>
+    </row>
+    <row r="3866">
+      <c r="A3866" s="3" t="n">
+        <v>45255</v>
+      </c>
+      <c r="B3866" t="n">
+        <v>37809.85286625321</v>
+      </c>
+    </row>
+    <row r="3867">
+      <c r="A3867" s="3" t="n">
+        <v>45256</v>
+      </c>
+      <c r="B3867" t="n">
+        <v>37491.83818600814</v>
+      </c>
+    </row>
+    <row r="3868">
+      <c r="A3868" s="3" t="n">
+        <v>45257</v>
+      </c>
+      <c r="B3868" t="n">
+        <v>37250.16905148115</v>
+      </c>
+    </row>
+    <row r="3869">
+      <c r="A3869" s="3" t="n">
+        <v>45258</v>
+      </c>
+      <c r="B3869" t="n">
+        <v>37802.23604377473</v>
       </c>
     </row>
   </sheetData>
@@ -29532,7 +31403,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:B5"/>
+  <dimension ref="A1:B6"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -29546,10 +31417,8 @@
           <t>Property</t>
         </is>
       </c>
-      <c r="B1" s="1" t="inlineStr">
-        <is>
-          <t>Value</t>
-        </is>
+      <c r="B1" s="1" t="n">
+        <v>0</v>
       </c>
     </row>
     <row r="2">
@@ -29584,7 +31453,7 @@
       </c>
       <c r="B4" t="inlineStr">
         <is>
-          <t>Bitcoin</t>
+          <t xml:space="preserve"> Bitcoin (USD)</t>
         </is>
       </c>
     </row>
@@ -29596,115 +31465,19 @@
       </c>
       <c r="B5" t="inlineStr">
         <is>
-          <t>BTC</t>
+          <t>Trace_2</t>
         </is>
       </c>
     </row>
-  </sheetData>
-  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <sheetPr>
-    <outlinePr summaryBelow="1" summaryRight="1"/>
-    <pageSetUpPr/>
-  </sheetPr>
-  <dimension ref="A1:B8"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A1" sqref="A1"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
-  <sheetData>
-    <row r="1">
-      <c r="B1" s="1" t="n">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="2">
-      <c r="A2" s="1" t="inlineStr">
-        <is>
-          <t>Ticker</t>
-        </is>
-      </c>
-      <c r="B2" t="inlineStr">
-        <is>
-          <t>bitcoin</t>
-        </is>
-      </c>
-    </row>
-    <row r="3">
-      <c r="A3" s="1" t="inlineStr">
+    <row r="6">
+      <c r="A6" s="1" t="inlineStr">
         <is>
           <t>Source</t>
         </is>
       </c>
-      <c r="B3" t="inlineStr">
+      <c r="B6" t="inlineStr">
         <is>
           <t>coingecko</t>
-        </is>
-      </c>
-    </row>
-    <row r="4">
-      <c r="A4" s="1" t="inlineStr">
-        <is>
-          <t>UnitsType</t>
-        </is>
-      </c>
-      <c r="B4" t="inlineStr">
-        <is>
-          <t>yoy</t>
-        </is>
-      </c>
-    </row>
-    <row r="5">
-      <c r="A5" s="1" t="inlineStr">
-        <is>
-          <t>TraceColor</t>
-        </is>
-      </c>
-      <c r="B5" t="inlineStr">
-        <is>
-          <t>orangered</t>
-        </is>
-      </c>
-    </row>
-    <row r="6">
-      <c r="A6" s="1" t="inlineStr">
-        <is>
-          <t>Legend_Name</t>
-        </is>
-      </c>
-      <c r="B6" t="inlineStr">
-        <is>
-          <t>Bitcoin</t>
-        </is>
-      </c>
-    </row>
-    <row r="7">
-      <c r="A7" s="1" t="inlineStr">
-        <is>
-          <t>Name</t>
-        </is>
-      </c>
-      <c r="B7" t="inlineStr">
-        <is>
-          <t>BTC</t>
-        </is>
-      </c>
-    </row>
-    <row r="8">
-      <c r="A8" s="1" t="inlineStr">
-        <is>
-          <t>Axis</t>
-        </is>
-      </c>
-      <c r="B8" t="inlineStr">
-        <is>
-          <t>ax3</t>
         </is>
       </c>
     </row>

</xml_diff>